<commit_message>
Correciones en logica neruona.py
</commit_message>
<xml_diff>
--- a/src/data/EJEMPLO_1.xlsx
+++ b/src/data/EJEMPLO_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WORLD\PYTHOM\Base Radial\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WORLD\PYTHOM\Perceptron Multicapa\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70981DA0-25A7-4115-BB19-14247402E824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83492B23-9BA3-43CE-8663-E4CEC953DF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,12 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +394,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +415,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -424,18 +423,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -446,10 +445,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -457,6 +456,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>